<commit_message>
Schéma altium PréTPI terminé
</commit_message>
<xml_diff>
--- a/5-Hardware/1438-5100-Puit de courant/1438-5100-Puit de courant_BOM.xlsx
+++ b/5-Hardware/1438-5100-Puit de courant/1438-5100-Puit de courant_BOM.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BOM Simple'!$1:$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'BOM Simple'!$A$1:$J$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'BOM Simple'!$A$1:$J$50</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="196">
   <si>
     <t>Pos.</t>
   </si>
@@ -152,9 +152,6 @@
     <t>R11, R12, R21, R36</t>
   </si>
   <si>
-    <t>R15</t>
-  </si>
-  <si>
     <t>R16</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
     <t>RES 10kohm  ±1% 0.125W 2012 (0805 INCH)</t>
   </si>
   <si>
-    <t>RES 0ohm  ±1% 0.125W 2012 (0805 INCH)</t>
-  </si>
-  <si>
     <t>RES 1.8kohm  ±1% 0.125W 2012 (0805 INCH)</t>
   </si>
   <si>
@@ -368,10 +362,10 @@
     <t>PN-108075</t>
   </si>
   <si>
-    <t>PN-747862</t>
-  </si>
-  <si>
-    <t>PN-324029</t>
+    <t>KAM21AR81H104KU</t>
+  </si>
+  <si>
+    <t>KGM21AR51E105KU</t>
   </si>
   <si>
     <t>PN-514948</t>
@@ -425,9 +419,6 @@
     <t>PN-374909</t>
   </si>
   <si>
-    <t>PN-391869</t>
-  </si>
-  <si>
     <t>PN-653534</t>
   </si>
   <si>
@@ -515,10 +506,10 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
-    <t>FAB.0805_C 100n</t>
-  </si>
-  <si>
-    <t>FAB.0805_C 1u</t>
+    <t>581-KAM21AR81H104KU</t>
+  </si>
+  <si>
+    <t>581-KGM21AR51E105KU</t>
   </si>
   <si>
     <t>FAB.0603_C 10nF</t>
@@ -558,9 +549,6 @@
   </si>
   <si>
     <t>FAB.0805_R 10k</t>
-  </si>
-  <si>
-    <t>FAB.0805_R 0R</t>
   </si>
   <si>
     <t>FAB.0805_R 1K8</t>
@@ -1112,17 +1100,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1447,19 +1425,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:K50" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A4:K50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A4:K49" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A4:K49"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Pos." dataDxfId="30"/>
-    <tableColumn id="2" name="Designator" dataDxfId="29"/>
+    <tableColumn id="1" name="Pos." dataDxfId="29"/>
+    <tableColumn id="2" name="Designator" dataDxfId="28"/>
     <tableColumn id="3" name="Description"/>
-    <tableColumn id="4" name="PN" dataDxfId="28"/>
-    <tableColumn id="5" name="Quantity" dataDxfId="27"/>
-    <tableColumn id="6" name="Supplier 1" dataDxfId="26"/>
+    <tableColumn id="4" name="PN" dataDxfId="27"/>
+    <tableColumn id="5" name="Quantity" dataDxfId="26"/>
+    <tableColumn id="6" name="Supplier 1" dataDxfId="25"/>
     <tableColumn id="7" name="Supplier Part Number 1"/>
-    <tableColumn id="8" name="Supplier Price 1" dataDxfId="25"/>
-    <tableColumn id="9" name="Order Qty" dataDxfId="24"/>
-    <tableColumn id="10" name="Total" dataDxfId="23"/>
+    <tableColumn id="8" name="Supplier Price 1" dataDxfId="24"/>
+    <tableColumn id="9" name="Order Qty" dataDxfId="23"/>
+    <tableColumn id="10" name="Total" dataDxfId="22"/>
     <tableColumn id="11" name="IsStocked"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1732,7 +1710,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:C8"/>
@@ -1825,22 +1803,22 @@
         <v>18</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>7</v>
@@ -1849,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1861,16 +1839,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E5" s="28">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>17</v>
@@ -1899,30 +1877,30 @@
         <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E6" s="29">
         <v>6</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H6" s="24">
-        <v>0.02</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="I6" s="21">
-        <f t="shared" ref="I6:I49" si="0">$C$3*E6</f>
+        <f t="shared" ref="I6:I48" si="0">$C$3*E6</f>
         <v>6</v>
       </c>
       <c r="J6" s="24">
         <f>I6*H6</f>
-        <v>0.12</v>
+        <v>1.554</v>
       </c>
       <c r="K6" s="16">
         <v>1</v>
@@ -1937,22 +1915,22 @@
         <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E7" s="28">
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H7" s="23">
-        <v>2.23E-2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="20">
         <f>$C$3*E7</f>
@@ -1960,7 +1938,7 @@
       </c>
       <c r="J7" s="23">
         <f>H7*I7</f>
-        <v>0.15610000000000002</v>
+        <v>7</v>
       </c>
       <c r="K7" s="15">
         <v>1</v>
@@ -1975,10 +1953,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="29">
         <v>1</v>
@@ -1987,7 +1965,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H8" s="24">
         <v>1.23E-2</v>
@@ -2013,19 +1991,19 @@
         <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E9" s="28">
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H9" s="23">
         <v>0.35399999999999998</v>
@@ -2051,19 +2029,19 @@
         <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E10" s="29">
         <v>2</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H10" s="24">
         <v>4.57</v>
@@ -2089,16 +2067,16 @@
         <v>24</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E11" s="28">
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G11" s="5">
         <v>3517015</v>
@@ -2127,19 +2105,19 @@
         <v>25</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E12" s="29">
         <v>2</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H12" s="24">
         <v>1.33</v>
@@ -2165,19 +2143,19 @@
         <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E13" s="28">
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H13" s="23">
         <v>1.26</v>
@@ -2203,19 +2181,19 @@
         <v>27</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E14" s="29">
         <v>1</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H14" s="24">
         <v>0.65800000000000003</v>
@@ -2241,19 +2219,19 @@
         <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E15" s="28">
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H15" s="23">
         <v>0.83</v>
@@ -2279,19 +2257,19 @@
         <v>29</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E16" s="29">
         <v>4</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H16" s="24">
         <v>8.5999999999999993E-2</v>
@@ -2317,16 +2295,16 @@
         <v>30</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E17" s="28">
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G17" s="5">
         <v>9306803</v>
@@ -2355,19 +2333,19 @@
         <v>31</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" s="29">
         <v>1</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H18" s="24">
         <v>8.5999999999999993E-2</v>
@@ -2393,10 +2371,10 @@
         <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E19" s="28">
         <v>1</v>
@@ -2405,7 +2383,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H19" s="23">
         <v>0.02</v>
@@ -2431,16 +2409,16 @@
         <v>33</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E20" s="29">
         <v>2</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G20" s="8">
         <v>9353801</v>
@@ -2469,16 +2447,16 @@
         <v>34</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E21" s="28">
         <v>2</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G21" s="5">
         <v>3399704</v>
@@ -2507,10 +2485,10 @@
         <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E22" s="29">
         <v>3</v>
@@ -2519,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H22" s="24">
         <v>0.02</v>
@@ -2545,10 +2523,10 @@
         <v>36</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E23" s="28">
         <v>2</v>
@@ -2557,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H23" s="23">
         <v>0.02</v>
@@ -2583,19 +2561,19 @@
         <v>37</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E24" s="29">
         <v>4</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G24" s="8">
-        <v>3399704</v>
+        <v>3399699</v>
       </c>
       <c r="H24" s="24">
         <v>0.15</v>
@@ -2621,10 +2599,10 @@
         <v>38</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E25" s="28">
         <v>4</v>
@@ -2633,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H25" s="23">
         <v>0.02</v>
@@ -2659,10 +2637,10 @@
         <v>39</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E26" s="29">
         <v>1</v>
@@ -2671,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H26" s="24">
         <v>0.02</v>
@@ -2697,30 +2675,30 @@
         <v>40</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E27" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H27" s="23">
         <v>0.02</v>
       </c>
       <c r="I27" s="20">
         <f>$C$3*E27</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="23">
         <f>H27*I27</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K27" s="15">
         <v>1</v>
@@ -2735,10 +2713,10 @@
         <v>41</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E28" s="29">
         <v>2</v>
@@ -2747,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H28" s="24">
         <v>0.02</v>
@@ -2773,30 +2751,30 @@
         <v>42</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E29" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H29" s="23">
-        <v>0.02</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="I29" s="20">
         <f>$C$3*E29</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" s="23">
         <f>H29*I29</f>
-        <v>0.04</v>
+        <v>0.41700000000000004</v>
       </c>
       <c r="K29" s="15">
         <v>1</v>
@@ -2811,30 +2789,30 @@
         <v>43</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H30" s="24">
-        <v>0.13900000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" ref="I30:I36" si="12">$C$3*E30</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" s="24">
         <f>I30*H30</f>
-        <v>0.41700000000000004</v>
+        <v>0.04</v>
       </c>
       <c r="K30" s="16">
         <v>1</v>
@@ -2849,10 +2827,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E31" s="28">
         <v>2</v>
@@ -2861,7 +2839,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H31" s="23">
         <v>0.02</v>
@@ -2878,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <f>ROW(A32) - ROW($A$4)</f>
         <v>28</v>
@@ -2887,22 +2865,22 @@
         <v>45</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E32" s="29">
         <v>2</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H32" s="24">
-        <v>0.02</v>
+        <v>0.623</v>
       </c>
       <c r="I32" s="21">
         <f t="shared" ref="I32" si="13">$C$3*E32</f>
@@ -2910,13 +2888,13 @@
       </c>
       <c r="J32" s="24">
         <f>I32*H32</f>
-        <v>0.04</v>
+        <v>1.246</v>
       </c>
       <c r="K32" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
         <f>ROW(A33) - ROW($A$4)</f>
         <v>29</v>
@@ -2925,30 +2903,30 @@
         <v>46</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E33" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H33" s="23">
-        <v>0.623</v>
+        <v>0.02</v>
       </c>
       <c r="I33" s="20">
         <f>$C$3*E33</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" s="23">
         <f>H33*I33</f>
-        <v>1.246</v>
+        <v>0.02</v>
       </c>
       <c r="K33" s="15">
         <v>1</v>
@@ -2963,10 +2941,10 @@
         <v>47</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E34" s="29">
         <v>1</v>
@@ -2975,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H34" s="24">
         <v>0.02</v>
@@ -3001,22 +2979,22 @@
         <v>48</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E35" s="28">
         <v>1</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H35" s="23">
-        <v>0.02</v>
+        <v>2.12</v>
       </c>
       <c r="I35" s="20">
         <f>$C$3*E35</f>
@@ -3024,7 +3002,7 @@
       </c>
       <c r="J35" s="23">
         <f>H35*I35</f>
-        <v>0.02</v>
+        <v>2.12</v>
       </c>
       <c r="K35" s="15">
         <v>1</v>
@@ -3039,22 +3017,22 @@
         <v>49</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E36" s="29">
         <v>1</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H36" s="24">
-        <v>2.12</v>
+        <v>0.02</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" ref="I36" si="15">$C$3*E36</f>
@@ -3062,13 +3040,13 @@
       </c>
       <c r="J36" s="24">
         <f>I36*H36</f>
-        <v>2.12</v>
+        <v>0.02</v>
       </c>
       <c r="K36" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <f>ROW(A37) - ROW($A$4)</f>
         <v>33</v>
@@ -3077,22 +3055,22 @@
         <v>50</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37" s="28">
         <v>1</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H37" s="23">
-        <v>0.02</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="I37" s="20">
         <f>$C$3*E37</f>
@@ -3100,13 +3078,11 @@
       </c>
       <c r="J37" s="23">
         <f>H37*I37</f>
-        <v>0.02</v>
-      </c>
-      <c r="K37" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="27">
         <f>ROW(A38) - ROW($A$4)</f>
         <v>34</v>
@@ -3115,32 +3091,34 @@
         <v>51</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E38" s="29">
         <v>1</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>156</v>
+        <v>2</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H38" s="24">
-        <v>2.5299999999999998</v>
+        <v>0.02</v>
       </c>
       <c r="I38" s="21">
-        <f t="shared" ref="I38:I49" si="16">$C$3*E38</f>
+        <f t="shared" ref="I38:I48" si="16">$C$3*E38</f>
         <v>1</v>
       </c>
       <c r="J38" s="24">
         <f>I38*H38</f>
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="K38" s="16"/>
+        <v>0.02</v>
+      </c>
+      <c r="K38" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
@@ -3151,10 +3129,10 @@
         <v>52</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E39" s="28">
         <v>1</v>
@@ -3163,7 +3141,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H39" s="23">
         <v>0.02</v>
@@ -3189,10 +3167,10 @@
         <v>53</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E40" s="29">
         <v>1</v>
@@ -3201,7 +3179,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H40" s="24">
         <v>0.02</v>
@@ -3227,30 +3205,30 @@
         <v>54</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E41" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H41" s="23">
         <v>0.02</v>
       </c>
       <c r="I41" s="20">
         <f>$C$3*E41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J41" s="23">
         <f>H41*I41</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K41" s="15">
         <v>1</v>
@@ -3265,22 +3243,22 @@
         <v>55</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E42" s="29">
         <v>2</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H42" s="24">
-        <v>0.02</v>
+        <v>0.33</v>
       </c>
       <c r="I42" s="21">
         <f t="shared" ref="I42:I44" si="18">$C$3*E42</f>
@@ -3288,7 +3266,7 @@
       </c>
       <c r="J42" s="24">
         <f>I42*H42</f>
-        <v>0.04</v>
+        <v>0.66</v>
       </c>
       <c r="K42" s="16">
         <v>1</v>
@@ -3303,30 +3281,30 @@
         <v>56</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E43" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>158</v>
+        <v>2</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H43" s="23">
-        <v>0.33</v>
+        <v>0.02</v>
       </c>
       <c r="I43" s="20">
         <f>$C$3*E43</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43" s="23">
         <f>H43*I43</f>
-        <v>0.66</v>
+        <v>0.02</v>
       </c>
       <c r="K43" s="15">
         <v>1</v>
@@ -3341,10 +3319,10 @@
         <v>57</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E44" s="29">
         <v>1</v>
@@ -3353,7 +3331,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H44" s="24">
         <v>0.02</v>
@@ -3379,10 +3357,10 @@
         <v>58</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E45" s="28">
         <v>1</v>
@@ -3391,10 +3369,10 @@
         <v>2</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H45" s="23">
-        <v>0.02</v>
+        <v>1.7</v>
       </c>
       <c r="I45" s="20">
         <f>$C$3*E45</f>
@@ -3402,9 +3380,9 @@
       </c>
       <c r="J45" s="23">
         <f>H45*I45</f>
-        <v>0.02</v>
-      </c>
-      <c r="K45" s="15">
+        <v>1.7</v>
+      </c>
+      <c r="K45" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3417,10 +3395,10 @@
         <v>59</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E46" s="29">
         <v>1</v>
@@ -3429,18 +3407,18 @@
         <v>2</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H46" s="24">
-        <v>1.7</v>
+        <v>1.51</v>
       </c>
       <c r="I46" s="21">
-        <f t="shared" ref="I46:I49" si="20">$C$3*E46</f>
+        <f t="shared" ref="I46:I48" si="20">$C$3*E46</f>
         <v>1</v>
       </c>
       <c r="J46" s="24">
         <f>I46*H46</f>
-        <v>1.7</v>
+        <v>1.51</v>
       </c>
       <c r="K46" s="16" t="b">
         <v>1</v>
@@ -3455,30 +3433,30 @@
         <v>60</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E47" s="28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H47" s="23">
-        <v>1.51</v>
+        <v>0.04</v>
       </c>
       <c r="I47" s="20">
         <f>$C$3*E47</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J47" s="23">
         <f>H47*I47</f>
-        <v>1.51</v>
+        <v>0.2</v>
       </c>
       <c r="K47" s="15" t="b">
         <v>1</v>
@@ -3493,87 +3471,49 @@
         <v>61</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>152</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D48" s="10"/>
       <c r="E48" s="29">
-        <v>5</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="H48" s="24">
-        <v>0.04</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="24"/>
       <c r="I48" s="21">
         <f t="shared" ref="I48" si="21">$C$3*E48</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J48" s="24">
         <f>I48*H48</f>
-        <v>0.2</v>
-      </c>
-      <c r="K48" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="26">
-        <f>ROW(A49) - ROW($A$4)</f>
-        <v>45</v>
-      </c>
-      <c r="B49" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>108</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="6"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="28">
-        <v>2</v>
-      </c>
+      <c r="E49" s="28"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="23"/>
-      <c r="I49" s="20">
-        <f>$C$3*E49</f>
-        <v>2</v>
-      </c>
-      <c r="J49" s="23">
-        <f>H49*I49</f>
-        <v>0</v>
-      </c>
+      <c r="I49" s="20"/>
+      <c r="J49" s="23"/>
       <c r="K49" s="15"/>
     </row>
     <row r="50" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="15"/>
-    </row>
-    <row r="51" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H51" s="11" t="s">
+      <c r="H50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I51" s="22">
-        <f>SUM(I5:I49)</f>
-        <v>86</v>
-      </c>
-      <c r="J51" s="25">
-        <f>SUM(J5:J49)</f>
-        <v>36.683400000000006</v>
+      <c r="I50" s="22">
+        <f>SUM(I5:I48)</f>
+        <v>85</v>
+      </c>
+      <c r="J50" s="25">
+        <f>SUM(J5:J48)</f>
+        <v>44.94130000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3591,7 +3531,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="23" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
+          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{64211BAB-4930-4668-885C-0EA0CE6E5BE5}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K5)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3605,10 +3545,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K5:K6 K50</xm:sqref>
+          <xm:sqref>K5:K6 K49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="22" operator="containsText" id="{299B62D8-3C8C-4FBB-9BFA-B984D48D2646}">
+          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{8921CBE3-D5A3-4832-ADB5-6868A6547FF9}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K7)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3625,7 +3565,7 @@
           <xm:sqref>K7:K8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="21" operator="containsText" id="{4BB68733-3DB3-4E05-A220-7F57FFD79C87}">
+          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{EDE89604-4942-443C-A10E-36C6F65EFFCA}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K9)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3642,7 +3582,7 @@
           <xm:sqref>K9:K10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="20" operator="containsText" id="{4B811CC4-7C72-4E89-88AF-A64CC3E11029}">
+          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{D9DB4EB3-9E8F-4837-9D44-B0C1F2BB6568}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K11)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3659,7 +3599,7 @@
           <xm:sqref>K11:K12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="19" operator="containsText" id="{8046AAE9-5FB0-46FC-9D12-A14A1AF86527}">
+          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{9887E96A-3F52-4205-BB83-8BFFAF62ABD0}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K13)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3676,7 +3616,7 @@
           <xm:sqref>K13:K14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="18" operator="containsText" id="{CD4B7A84-167F-4F4E-865D-C9B8161EEC19}">
+          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{E5C332BD-9FCC-4187-81B2-1F6F7BC5A34D}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K15)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3693,7 +3633,7 @@
           <xm:sqref>K15:K16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="17" operator="containsText" id="{A32C1268-1509-4A2D-997A-563AD33517AA}">
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{10137E28-36AC-45EA-AE5B-0345BA4ADC15}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K17)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3710,7 +3650,7 @@
           <xm:sqref>K17:K18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{9A5D6654-D766-418A-8223-252178112F9F}">
+          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{D431BE87-9773-456A-A0A0-742379816AB7}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K19)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3727,7 +3667,7 @@
           <xm:sqref>K19:K20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="15" operator="containsText" id="{9D142FED-D5EC-4367-925F-EE12E812344F}">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{018CD4F0-949A-43C3-853F-CD8AA8688421}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K21)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3744,7 +3684,7 @@
           <xm:sqref>K21:K22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{CCF7478F-991F-422E-9322-190A1F9789ED}">
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{08306D23-5A2D-4D81-9381-27E371AA3763}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K23)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3761,7 +3701,7 @@
           <xm:sqref>K23:K24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{A70AB42F-C3FD-4357-A3BF-63B55315F78D}">
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{57C9CB25-B99F-46F2-9E12-25E9F738D3A8}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K25)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3778,7 +3718,7 @@
           <xm:sqref>K25:K26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{CFF4CA19-F37F-4457-9315-1CAE0F7578AC}">
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{147CA338-00FD-4341-9670-6C03B8857C99}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K27)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3795,7 +3735,7 @@
           <xm:sqref>K27:K28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{3AC99AC8-5347-4959-BC22-B5782A8915A9}">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{69A35CCB-44E6-4210-826B-7A55AE39D84A}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K29)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3812,7 +3752,7 @@
           <xm:sqref>K29:K30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{69A6AEF3-CD49-4E52-A64D-04D2D862931C}">
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{A39F83DA-A7B3-4564-80B0-3E7C74E3EC52}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K31)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3829,7 +3769,7 @@
           <xm:sqref>K31:K32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{87F69E60-E0BA-48D8-BA5C-B8445973B5F2}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{5AE14EB1-830C-4690-BDE6-7CC97B8BAB92}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K33)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3846,7 +3786,7 @@
           <xm:sqref>K33:K34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{350562E5-56CC-449D-9E1F-5B5E2E4F0136}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{AE58FB8C-ED21-4044-A21B-5AB370802009}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K35)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3863,7 +3803,7 @@
           <xm:sqref>K35:K36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{FF6D0F6B-3354-4801-8EB6-D3EC54E6B8BF}">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{6701A9C3-57C6-4221-A333-8D212015BD73}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K37)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3880,7 +3820,7 @@
           <xm:sqref>K37:K38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{1020C30A-360E-417C-825A-444EDCDCA370}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{BB5C1527-9FB7-405F-8B6A-D6D87CEED990}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K39)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3897,7 +3837,7 @@
           <xm:sqref>K39:K40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{5992AE42-ACF5-4F38-8293-48FEDD3C9816}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{DA167763-B18D-4B6D-9BF3-76CF81E63666}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K41)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3914,7 +3854,7 @@
           <xm:sqref>K41:K42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{172ACD7A-F2CC-47B0-91B1-54653136B2ED}">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{D4FD9886-DB74-4D60-B553-033071A9CF08}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K43)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3931,7 +3871,7 @@
           <xm:sqref>K43:K44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A2DE59F4-5F27-4BEC-AF11-A39ECCDDC589}">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{746FD4CE-4DA2-4A71-A444-B39B4EBC85E9}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K45)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3948,7 +3888,7 @@
           <xm:sqref>K45:K46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{C58F4B88-F05A-4A8D-8D30-2897B788F764}">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A20D9785-D2E4-419F-BD3E-1D95835935C7}">
             <xm:f>NOT(ISERROR(SEARCH("VRAI",K47)))</xm:f>
             <xm:f>"VRAI"</xm:f>
             <x14:dxf>
@@ -3963,23 +3903,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>K47:K48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{299120AA-8768-420B-9171-E828BEE07B8D}">
-            <xm:f>NOT(ISERROR(SEARCH("VRAI",K49)))</xm:f>
-            <xm:f>"VRAI"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>K49</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4245,13 +4168,13 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A056176-9FE1-4C5F-A929-245972C77676}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -4268,7 +4191,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{678B5630-D48B-4ECC-B755-0C220FFBD3DA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{470659B8-7CE9-4CBD-8A53-4A346E82F9ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>